<commit_message>
final updates to manuscript code
</commit_message>
<xml_diff>
--- a/Interpolat_Diff_Tax/Money_Analysis/Data/US_China_Group_Price_v1.xlsx
+++ b/Interpolat_Diff_Tax/Money_Analysis/Data/US_China_Group_Price_v1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amorgan/Documents/PostDoc/Diff_Tax_Analysis/Theoretical_Analysis/Interpolat_Diff_Tax/Money_Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amorgan/Documents/PostDoc/Diff_Tax_Analysis/Theoretical_Analysis/Interpolat_Diff_Tax/Money_Analysis/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FA907F-904E-9A44-8FAF-E50481AB7600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614A86CA-AD67-534B-B861-E59194D8DA15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4400" yWindow="4960" windowWidth="34520" windowHeight="14940" xr2:uid="{57EAA5CF-5E39-1A4F-9399-76395567C3D1}"/>
   </bookViews>
@@ -456,7 +456,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -860,52 +860,40 @@
         <v>20</v>
       </c>
       <c r="B10">
-        <f>B8*0.074202923</f>
-        <v>661343910.37778938</v>
+        <v>366444211.24861097</v>
       </c>
       <c r="C10">
-        <f t="shared" ref="C10:M11" si="2">C8*0.074202923</f>
-        <v>136486036.85512602</v>
+        <v>75625581.995992005</v>
       </c>
       <c r="D10">
-        <f t="shared" si="2"/>
-        <v>128145541.73984917</v>
+        <v>71004194.989956662</v>
       </c>
       <c r="E10">
-        <f t="shared" si="2"/>
-        <v>336334667.36711282</v>
+        <v>186359759.21892264</v>
       </c>
       <c r="F10">
-        <f t="shared" si="2"/>
-        <v>112735162.3763871</v>
+        <v>62465454.06821765</v>
       </c>
       <c r="G10">
-        <f t="shared" si="2"/>
-        <v>2220108160.9922957</v>
+        <v>1230140281.2897937</v>
       </c>
       <c r="H10">
-        <f t="shared" si="2"/>
-        <v>644473756.69682384</v>
+        <v>357096623.61340791</v>
       </c>
       <c r="I10">
-        <f t="shared" si="2"/>
-        <v>163788260.34374601</v>
+        <v>90753477.777032003</v>
       </c>
       <c r="J10">
-        <f t="shared" si="2"/>
-        <v>27124210.676343001</v>
+        <v>15029260.617756</v>
       </c>
       <c r="K10">
-        <f t="shared" si="2"/>
-        <v>4991609.1113623306</v>
+        <v>2765801.9299363601</v>
       </c>
       <c r="L10">
-        <f t="shared" si="2"/>
-        <v>12515047.18447848</v>
+        <v>6934465.5969321597</v>
       </c>
       <c r="M10">
-        <f t="shared" si="2"/>
-        <v>219821807.38606605</v>
+        <v>121801119.7484466</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -913,52 +901,40 @@
         <v>21</v>
       </c>
       <c r="B11">
-        <f>B9*0.074202923</f>
-        <v>92089494.551454663</v>
+        <v>51025890.865032718</v>
       </c>
       <c r="C11">
-        <f t="shared" si="2"/>
-        <v>10971279.969732456</v>
+        <v>6079079.2382131144</v>
       </c>
       <c r="D11">
-        <f t="shared" si="2"/>
-        <v>48027614.405588076</v>
+        <v>26611632.772054341</v>
       </c>
       <c r="E11">
-        <f t="shared" si="2"/>
-        <v>791466.91678207996</v>
+        <v>438544.10012470215</v>
       </c>
       <c r="F11">
-        <f t="shared" si="2"/>
-        <v>13648624.462331038</v>
+        <v>7562569.7118316786</v>
       </c>
       <c r="G11">
-        <f t="shared" si="2"/>
-        <v>47412900.491740361</v>
+        <v>26271025.787142672</v>
       </c>
       <c r="H11">
-        <f t="shared" si="2"/>
-        <v>16092839.617593616</v>
+        <v>8916885.493132893</v>
       </c>
       <c r="I11">
-        <f t="shared" si="2"/>
-        <v>3871651.112200113</v>
+        <v>2145244.1245425958</v>
       </c>
       <c r="J11">
-        <f t="shared" si="2"/>
-        <v>5475187.3344656406</v>
+        <v>3033747.90745488</v>
       </c>
       <c r="K11">
-        <f t="shared" si="2"/>
-        <v>1551309.0519142926</v>
+        <v>859565.21714523504</v>
       </c>
       <c r="L11">
-        <f t="shared" si="2"/>
-        <v>9270764.7937740013</v>
+        <v>5136840.3628080003</v>
       </c>
       <c r="M11">
-        <f t="shared" si="2"/>
-        <v>11728677.101964157</v>
+        <v>6498745.6029703859</v>
       </c>
     </row>
   </sheetData>

</xml_diff>